<commit_message>
fixed bug of courses analyzer
</commit_message>
<xml_diff>
--- a/api/python/TaiGer_Transcript-Program_Comparer/ME_Programs.xlsx
+++ b/api/python/TaiGer_Transcript-Program_Comparer/ME_Programs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\OneDrive\20110706\TaiGer_Transcript-Program_Comparer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2BCF949-416D-4C6D-BF36-6BF20D179C63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F947629-BADC-466B-9326-C7F5BDC7DA2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-6975" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
   <si>
     <t>Program</t>
   </si>
@@ -46,6 +46,12 @@
   </si>
   <si>
     <t>TU_DORTMUND_MANUFACTURING_TECH</t>
+  </si>
+  <si>
+    <t>TUM_MW</t>
+  </si>
+  <si>
+    <t>TU_CHEMNITZ_ADVANCED_MANUFACTURING</t>
   </si>
 </sst>
 </file>
@@ -363,10 +369,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -392,7 +398,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
@@ -400,7 +406,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
@@ -408,15 +414,31 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B6" xr:uid="{610A300D-EA49-404E-A3AA-32352271D928}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B7" xr:uid="{610A300D-EA49-404E-A3AA-32352271D928}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
update course analyser. import rich text editor(default setting, not backend wiring). add react quill and style.css.
</commit_message>
<xml_diff>
--- a/api/python/TaiGer_Transcript-Program_Comparer/ME_Programs.xlsx
+++ b/api/python/TaiGer_Transcript-Program_Comparer/ME_Programs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\OneDrive\20110706\TaiGer_Transcript-Program_Comparer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F947629-BADC-466B-9326-C7F5BDC7DA2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D240C7B-B2B4-402B-B58F-73A0F5FE1D6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6975" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21825" yWindow="-16350" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Program_choosing" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
   <si>
     <t>Program</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>TU_CHEMNITZ_ADVANCED_MANUFACTURING</t>
+  </si>
+  <si>
+    <t>TUM_COMPUTATIONAL_MECHANICS</t>
   </si>
 </sst>
 </file>
@@ -369,10 +372,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -436,9 +439,17 @@
         <v>2</v>
       </c>
     </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B7" xr:uid="{610A300D-EA49-404E-A3AA-32352271D928}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B8" xr:uid="{610A300D-EA49-404E-A3AA-32352271D928}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>